<commit_message>
Community - aggregator control remaining capacity of households
</commit_message>
<xml_diff>
--- a/data/input_community/CommunityScenario.xlsx
+++ b/data/input_community/CommunityScenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_community/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9405A830-E1C4-1E4D-A04B-B83D8B2959CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAFBB24-3E29-CA4D-8390-706A8ABDC52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31480" yWindow="-10080" windowWidth="26000" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
   <si>
     <t>ID_Scenario</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>aggregator_battery_discharge_efficiency</t>
+  </si>
+  <si>
+    <t>aggregator_household_battery_control</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -445,14 +448,14 @@
     <col min="2" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,19 +478,22 @@
         <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -521,8 +527,11 @@
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -556,8 +565,11 @@
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -591,8 +603,11 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -626,8 +641,11 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -661,8 +679,11 @@
       <c r="K6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -696,8 +717,11 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -731,8 +755,11 @@
       <c r="K8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -766,8 +793,11 @@
       <c r="K9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -801,8 +831,11 @@
       <c r="K10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -836,8 +869,11 @@
       <c r="K11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -871,8 +907,11 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -906,8 +945,11 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -941,8 +983,11 @@
       <c r="K14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -976,8 +1021,11 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1011,8 +1059,11 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1046,8 +1097,11 @@
       <c r="K17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1081,8 +1135,11 @@
       <c r="K18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1116,8 +1173,11 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1151,8 +1211,11 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1186,8 +1249,11 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1221,8 +1287,11 @@
       <c r="K22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1256,8 +1325,11 @@
       <c r="K23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1291,8 +1363,11 @@
       <c r="K24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1326,8 +1401,11 @@
       <c r="K25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1361,8 +1439,11 @@
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1396,8 +1477,11 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1431,8 +1515,11 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1466,8 +1553,11 @@
       <c r="K29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1501,8 +1591,11 @@
       <c r="K30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1534,6 +1627,9 @@
         <v>1</v>
       </c>
       <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Community - analyzer updated
</commit_message>
<xml_diff>
--- a/data/input_community/CommunityScenario.xlsx
+++ b/data/input_community/CommunityScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_community/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAFBB24-3E29-CA4D-8390-706A8ABDC52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD31056-8EC2-834E-A5CA-CC6CCD4B63F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -981,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1285,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1399,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27">
         <v>1</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <v>1</v>
@@ -1551,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L29">
         <v>1</v>
@@ -1589,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30">
         <v>1</v>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L31">
         <v>1</v>

</xml_diff>